<commit_message>
Completed Lesson 12 JMeter
</commit_message>
<xml_diff>
--- a/Katalon Projects/Coolmate Test/Data Files/COOLMATE-002/SearchKeywords.xlsx
+++ b/Katalon Projects/Coolmate Test/Data Files/COOLMATE-002/SearchKeywords.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="7665"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Search Keywords" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>